<commit_message>
skill score file changes
</commit_message>
<xml_diff>
--- a/AdditionalFiles/SKillScoreCalculations.xlsx
+++ b/AdditionalFiles/SKillScoreCalculations.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dw1537\ProjectSolarPV\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dw1537\ProjectSolarPV\AdditionalFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9F4C4B5B-C528-4D31-9D98-2569D2B0296B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA24A10E-EDFD-4915-9F77-A5065D25668B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{4F7AE457-9BFF-4E59-B6C5-4349FA28ED9F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="16">
   <si>
     <t>CNN</t>
   </si>
@@ -55,6 +55,33 @@
   </si>
   <si>
     <t>Skill score</t>
+  </si>
+  <si>
+    <t>CNN Pretrained</t>
+  </si>
+  <si>
+    <t>LSTM Preatrained</t>
+  </si>
+  <si>
+    <t>CNNLSTM pre</t>
+  </si>
+  <si>
+    <t>Simple Trans</t>
+  </si>
+  <si>
+    <t>Forecast Trans</t>
+  </si>
+  <si>
+    <t>SS simple</t>
+  </si>
+  <si>
+    <t>SS forecast</t>
+  </si>
+  <si>
+    <t>SS Simple</t>
+  </si>
+  <si>
+    <t>SS Forecast</t>
   </si>
 </sst>
 </file>
@@ -237,7 +264,12 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="7">
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FFFF0000"/>
@@ -255,17 +287,17 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FFFF0000"/>
       </font>
     </dxf>
     <dxf>
       <font>
         <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
       </font>
     </dxf>
   </dxfs>
@@ -578,10 +610,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B733F1F2-3B39-40A2-9C23-9B37E8224527}">
-  <dimension ref="B2:J42"/>
+  <dimension ref="B2:AD42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M39" sqref="M39"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="AH11" sqref="AH11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -592,9 +624,19 @@
     <col min="8" max="8" width="19" customWidth="1"/>
     <col min="9" max="9" width="25" customWidth="1"/>
     <col min="10" max="10" width="16" customWidth="1"/>
+    <col min="12" max="12" width="9.42578125" customWidth="1"/>
+    <col min="13" max="15" width="18.42578125" customWidth="1"/>
+    <col min="17" max="17" width="18.42578125" customWidth="1"/>
+    <col min="18" max="19" width="18.28515625" customWidth="1"/>
+    <col min="20" max="20" width="18.5703125" customWidth="1"/>
+    <col min="23" max="23" width="18.28515625" customWidth="1"/>
+    <col min="27" max="27" width="18.140625" customWidth="1"/>
+    <col min="28" max="28" width="18.28515625" customWidth="1"/>
+    <col min="29" max="29" width="14" customWidth="1"/>
+    <col min="30" max="30" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -613,8 +655,38 @@
       <c r="J2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M2" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>10</v>
+      </c>
+      <c r="R2" t="s">
+        <v>11</v>
+      </c>
+      <c r="S2" t="s">
+        <v>12</v>
+      </c>
+      <c r="T2" t="s">
+        <v>13</v>
+      </c>
+      <c r="W2" t="s">
+        <v>7</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B3" s="1">
         <v>1.485E-3</v>
       </c>
@@ -635,8 +707,44 @@
         <f>ROUND((I3 - H3) / (-H3), 4)</f>
         <v>0.8135</v>
       </c>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M3" s="1">
+        <v>2.3400000000000001E-3</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>2.5999999999999998E-4</v>
+      </c>
+      <c r="R3" s="1">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="S3">
+        <f>ROUND((Q3 - M3) / (-M3), 4)</f>
+        <v>0.88890000000000002</v>
+      </c>
+      <c r="T3">
+        <f>ROUND((R3 - M3) / (-M3), 4)</f>
+        <v>0.67949999999999999</v>
+      </c>
+      <c r="W3" s="1">
+        <v>2.3400000000000001E-3</v>
+      </c>
+      <c r="X3" s="1"/>
+      <c r="Y3" s="1"/>
+      <c r="AA3" s="1">
+        <v>2.3000000000000001E-4</v>
+      </c>
+      <c r="AB3" s="9">
+        <v>2.5000000000000001E-4</v>
+      </c>
+      <c r="AC3">
+        <f>ROUND((AA3 - W3) / (-W3), 4)</f>
+        <v>0.90169999999999995</v>
+      </c>
+      <c r="AD3">
+        <f>ROUND((AB3 - W3) / (-W3), 4)</f>
+        <v>0.89319999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B4" s="2">
         <v>3.3709999999999999E-3</v>
       </c>
@@ -657,8 +765,44 @@
         <f t="shared" ref="J4:J42" si="1">ROUND((I4 - H4) / (-H4), 4)</f>
         <v>0.92730000000000001</v>
       </c>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M4" s="2">
+        <v>3.1900000000000001E-3</v>
+      </c>
+      <c r="Q4" s="2">
+        <v>3.6000000000000002E-4</v>
+      </c>
+      <c r="R4" s="2">
+        <v>4.8999999999999998E-4</v>
+      </c>
+      <c r="S4">
+        <f t="shared" ref="S4:S33" si="2">ROUND((Q4 - M4) / (-M4), 4)</f>
+        <v>0.8871</v>
+      </c>
+      <c r="T4">
+        <f t="shared" ref="T4:T33" si="3">ROUND((R4 - M4) / (-M4), 4)</f>
+        <v>0.84640000000000004</v>
+      </c>
+      <c r="W4" s="2">
+        <v>3.1900000000000001E-3</v>
+      </c>
+      <c r="X4" s="2"/>
+      <c r="Y4" s="13"/>
+      <c r="AA4" s="2">
+        <v>5.5000000000000003E-4</v>
+      </c>
+      <c r="AB4" s="2">
+        <v>3.6999999999999999E-4</v>
+      </c>
+      <c r="AC4">
+        <f t="shared" ref="AC4:AC33" si="4">ROUND((AA4 - W4) / (-W4), 4)</f>
+        <v>0.8276</v>
+      </c>
+      <c r="AD4">
+        <f t="shared" ref="AD4:AD33" si="5">ROUND((AB4 - W4) / (-W4), 4)</f>
+        <v>0.88400000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="3">
         <v>3.0890000000000002E-3</v>
       </c>
@@ -679,8 +823,44 @@
         <f t="shared" si="1"/>
         <v>0.91739999999999999</v>
       </c>
-    </row>
-    <row r="6" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M5" s="4">
+        <v>1.99E-3</v>
+      </c>
+      <c r="Q5" s="4">
+        <v>1.8000000000000001E-4</v>
+      </c>
+      <c r="R5" s="4">
+        <v>1.0200000000000001E-3</v>
+      </c>
+      <c r="S5">
+        <f t="shared" si="2"/>
+        <v>0.90949999999999998</v>
+      </c>
+      <c r="T5">
+        <f t="shared" si="3"/>
+        <v>0.4874</v>
+      </c>
+      <c r="W5" s="4">
+        <v>1.99E-3</v>
+      </c>
+      <c r="X5" s="4"/>
+      <c r="Y5" s="4"/>
+      <c r="AA5" s="4">
+        <v>1E-4</v>
+      </c>
+      <c r="AB5" s="11">
+        <v>6.9999999999999994E-5</v>
+      </c>
+      <c r="AC5">
+        <f t="shared" si="4"/>
+        <v>0.94969999999999999</v>
+      </c>
+      <c r="AD5">
+        <f t="shared" si="5"/>
+        <v>0.96479999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="4">
         <v>1.207E-3</v>
       </c>
@@ -701,8 +881,44 @@
         <f t="shared" si="1"/>
         <v>0.77959999999999996</v>
       </c>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M6" s="1">
+        <v>3.9899999999999998E-2</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>1.4E-2</v>
+      </c>
+      <c r="R6" s="1">
+        <v>1.7299999999999999E-2</v>
+      </c>
+      <c r="S6">
+        <f t="shared" si="2"/>
+        <v>0.64910000000000001</v>
+      </c>
+      <c r="T6">
+        <f t="shared" si="3"/>
+        <v>0.56640000000000001</v>
+      </c>
+      <c r="W6" s="1">
+        <v>3.9899999999999998E-2</v>
+      </c>
+      <c r="X6" s="1"/>
+      <c r="Y6" s="1"/>
+      <c r="AA6" s="1">
+        <v>1.1900000000000001E-2</v>
+      </c>
+      <c r="AB6" s="1">
+        <v>9.9000000000000008E-3</v>
+      </c>
+      <c r="AC6">
+        <f t="shared" si="4"/>
+        <v>0.70179999999999998</v>
+      </c>
+      <c r="AD6">
+        <f t="shared" si="5"/>
+        <v>0.75190000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>2.7099999999999999E-2</v>
       </c>
@@ -723,8 +939,44 @@
         <f t="shared" si="1"/>
         <v>0.54610000000000003</v>
       </c>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M7" s="2">
+        <v>4.6300000000000001E-2</v>
+      </c>
+      <c r="Q7" s="2">
+        <v>1.5599999999999999E-2</v>
+      </c>
+      <c r="R7" s="13">
+        <v>1.2800000000000001E-2</v>
+      </c>
+      <c r="S7">
+        <f t="shared" si="2"/>
+        <v>0.66310000000000002</v>
+      </c>
+      <c r="T7">
+        <f t="shared" si="3"/>
+        <v>0.72350000000000003</v>
+      </c>
+      <c r="W7" s="2">
+        <v>4.6300000000000001E-2</v>
+      </c>
+      <c r="X7" s="2"/>
+      <c r="Y7" s="2"/>
+      <c r="AA7" s="2">
+        <v>1.7500000000000002E-2</v>
+      </c>
+      <c r="AB7" s="2">
+        <v>1.43E-2</v>
+      </c>
+      <c r="AC7">
+        <f t="shared" si="4"/>
+        <v>0.622</v>
+      </c>
+      <c r="AD7">
+        <f t="shared" si="5"/>
+        <v>0.69110000000000005</v>
+      </c>
+    </row>
+    <row r="8" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="2">
         <v>4.9099999999999998E-2</v>
       </c>
@@ -745,8 +997,44 @@
         <f t="shared" si="1"/>
         <v>0.74539999999999995</v>
       </c>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M8" s="4">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="Q8" s="4">
+        <v>1.2500000000000001E-2</v>
+      </c>
+      <c r="R8" s="4">
+        <v>2.35E-2</v>
+      </c>
+      <c r="S8">
+        <f t="shared" si="2"/>
+        <v>0.67110000000000003</v>
+      </c>
+      <c r="T8">
+        <f t="shared" si="3"/>
+        <v>0.38159999999999999</v>
+      </c>
+      <c r="W8" s="4">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="X8" s="4"/>
+      <c r="Y8" s="4"/>
+      <c r="AA8" s="4">
+        <v>9.4999999999999998E-3</v>
+      </c>
+      <c r="AB8" s="11">
+        <v>6.4000000000000003E-3</v>
+      </c>
+      <c r="AC8">
+        <f t="shared" si="4"/>
+        <v>0.75</v>
+      </c>
+      <c r="AD8">
+        <f t="shared" si="5"/>
+        <v>0.83160000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B9" s="3">
         <v>4.2299999999999997E-2</v>
       </c>
@@ -767,8 +1055,44 @@
         <f t="shared" si="1"/>
         <v>0.69979999999999998</v>
       </c>
-    </row>
-    <row r="10" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M9" s="5">
+        <v>3.0300000000000001E-2</v>
+      </c>
+      <c r="Q9" s="5">
+        <v>1.0800000000000001E-2</v>
+      </c>
+      <c r="R9" s="5">
+        <v>1.29E-2</v>
+      </c>
+      <c r="S9">
+        <f t="shared" si="2"/>
+        <v>0.64359999999999995</v>
+      </c>
+      <c r="T9">
+        <f t="shared" si="3"/>
+        <v>0.57430000000000003</v>
+      </c>
+      <c r="W9" s="5">
+        <v>3.0300000000000001E-2</v>
+      </c>
+      <c r="X9" s="5"/>
+      <c r="Y9" s="5"/>
+      <c r="AA9" s="5">
+        <v>9.4000000000000004E-3</v>
+      </c>
+      <c r="AB9" s="14">
+        <v>6.4999999999999997E-3</v>
+      </c>
+      <c r="AC9">
+        <f t="shared" si="4"/>
+        <v>0.68979999999999997</v>
+      </c>
+      <c r="AD9">
+        <f t="shared" si="5"/>
+        <v>0.78549999999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="4">
         <v>2.4400000000000002E-2</v>
       </c>
@@ -789,8 +1113,44 @@
         <f t="shared" si="1"/>
         <v>0.52049999999999996</v>
       </c>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M10" s="6">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="Q10" s="6">
+        <v>1.0800000000000001E-2</v>
+      </c>
+      <c r="R10" s="15">
+        <v>8.3999999999999995E-3</v>
+      </c>
+      <c r="S10">
+        <f t="shared" si="2"/>
+        <v>0.66249999999999998</v>
+      </c>
+      <c r="T10">
+        <f t="shared" si="3"/>
+        <v>0.73750000000000004</v>
+      </c>
+      <c r="W10" s="6">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="X10" s="6"/>
+      <c r="Y10" s="6"/>
+      <c r="AA10" s="6">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="AB10" s="6">
+        <v>9.1000000000000004E-3</v>
+      </c>
+      <c r="AC10">
+        <f t="shared" si="4"/>
+        <v>0.59379999999999999</v>
+      </c>
+      <c r="AD10">
+        <f t="shared" si="5"/>
+        <v>0.71560000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="5">
         <v>1.78E-2</v>
       </c>
@@ -811,8 +1171,44 @@
         <f t="shared" si="1"/>
         <v>0.52810000000000001</v>
       </c>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M11" s="8">
+        <v>3.0300000000000001E-2</v>
+      </c>
+      <c r="Q11" s="8">
+        <v>1.03E-2</v>
+      </c>
+      <c r="R11" s="8">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="S11">
+        <f t="shared" si="2"/>
+        <v>0.66010000000000002</v>
+      </c>
+      <c r="T11">
+        <f t="shared" si="3"/>
+        <v>0.40589999999999998</v>
+      </c>
+      <c r="W11" s="8">
+        <v>3.0300000000000001E-2</v>
+      </c>
+      <c r="X11" s="8"/>
+      <c r="Y11" s="8"/>
+      <c r="AA11" s="8">
+        <v>7.9000000000000008E-3</v>
+      </c>
+      <c r="AB11" s="12">
+        <v>4.4999999999999997E-3</v>
+      </c>
+      <c r="AC11">
+        <f t="shared" si="4"/>
+        <v>0.73929999999999996</v>
+      </c>
+      <c r="AD11">
+        <f t="shared" si="5"/>
+        <v>0.85150000000000003</v>
+      </c>
+    </row>
+    <row r="12" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B12" s="6">
         <v>2.9000000000000001E-2</v>
       </c>
@@ -834,7 +1230,7 @@
         <v>0.74829999999999997</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="7">
         <v>2.58E-2</v>
       </c>
@@ -855,8 +1251,20 @@
         <f t="shared" si="1"/>
         <v>0.68989999999999996</v>
       </c>
-    </row>
-    <row r="14" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M13" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>10</v>
+      </c>
+      <c r="R13" t="s">
+        <v>11</v>
+      </c>
+      <c r="W13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="8">
         <v>1.8700000000000001E-2</v>
       </c>
@@ -877,8 +1285,78 @@
         <f t="shared" si="1"/>
         <v>0.51339999999999997</v>
       </c>
-    </row>
-    <row r="16" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M14" s="1">
+        <v>3.2000000000000003E-4</v>
+      </c>
+      <c r="Q14" s="1">
+        <v>2.5999999999999998E-4</v>
+      </c>
+      <c r="R14" s="1">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="S14">
+        <f t="shared" si="2"/>
+        <v>0.1875</v>
+      </c>
+      <c r="T14">
+        <f t="shared" si="3"/>
+        <v>-1.3438000000000001</v>
+      </c>
+      <c r="W14" s="1">
+        <v>3.2000000000000003E-4</v>
+      </c>
+      <c r="AA14" s="1">
+        <v>2.3000000000000001E-4</v>
+      </c>
+      <c r="AB14" s="9">
+        <v>2.5000000000000001E-4</v>
+      </c>
+      <c r="AC14">
+        <f t="shared" si="4"/>
+        <v>0.28129999999999999</v>
+      </c>
+      <c r="AD14">
+        <f t="shared" si="5"/>
+        <v>0.21879999999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="M15" s="2">
+        <v>4.2999999999999999E-4</v>
+      </c>
+      <c r="Q15" s="2">
+        <v>3.6000000000000002E-4</v>
+      </c>
+      <c r="R15" s="2">
+        <v>4.8999999999999998E-4</v>
+      </c>
+      <c r="S15">
+        <f t="shared" si="2"/>
+        <v>0.1628</v>
+      </c>
+      <c r="T15">
+        <f t="shared" si="3"/>
+        <v>-0.13950000000000001</v>
+      </c>
+      <c r="W15" s="2">
+        <v>4.2999999999999999E-4</v>
+      </c>
+      <c r="AA15" s="2">
+        <v>5.5000000000000003E-4</v>
+      </c>
+      <c r="AB15" s="2">
+        <v>3.6999999999999999E-4</v>
+      </c>
+      <c r="AC15">
+        <f t="shared" si="4"/>
+        <v>-0.27910000000000001</v>
+      </c>
+      <c r="AD15">
+        <f t="shared" si="5"/>
+        <v>0.13950000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>3</v>
       </c>
@@ -888,8 +1366,42 @@
       <c r="H16" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M16" s="4">
+        <v>9.0000000000000006E-5</v>
+      </c>
+      <c r="Q16" s="4">
+        <v>1.8000000000000001E-4</v>
+      </c>
+      <c r="R16" s="4">
+        <v>1.0200000000000001E-3</v>
+      </c>
+      <c r="S16">
+        <f t="shared" si="2"/>
+        <v>-1</v>
+      </c>
+      <c r="T16">
+        <f t="shared" si="3"/>
+        <v>-10.333299999999999</v>
+      </c>
+      <c r="W16" s="4">
+        <v>9.0000000000000006E-5</v>
+      </c>
+      <c r="AA16" s="4">
+        <v>1E-4</v>
+      </c>
+      <c r="AB16" s="11">
+        <v>6.9999999999999994E-5</v>
+      </c>
+      <c r="AC16">
+        <f t="shared" si="4"/>
+        <v>-0.1111</v>
+      </c>
+      <c r="AD16">
+        <f t="shared" si="5"/>
+        <v>0.22220000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B17" s="1">
         <v>3.5199999999999999E-4</v>
       </c>
@@ -910,8 +1422,42 @@
         <f t="shared" si="1"/>
         <v>0.21310000000000001</v>
       </c>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M17" s="1">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="Q17" s="1">
+        <v>1.4E-2</v>
+      </c>
+      <c r="R17" s="1">
+        <v>1.7299999999999999E-2</v>
+      </c>
+      <c r="S17">
+        <f t="shared" si="2"/>
+        <v>-0.2727</v>
+      </c>
+      <c r="T17">
+        <f t="shared" si="3"/>
+        <v>-0.57269999999999999</v>
+      </c>
+      <c r="W17" s="1">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="AA17" s="1">
+        <v>1.1900000000000001E-2</v>
+      </c>
+      <c r="AB17" s="1">
+        <v>9.9000000000000008E-3</v>
+      </c>
+      <c r="AC17">
+        <f t="shared" si="4"/>
+        <v>-8.1799999999999998E-2</v>
+      </c>
+      <c r="AD17">
+        <f t="shared" si="5"/>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B18" s="2">
         <v>3.2699999999999998E-4</v>
       </c>
@@ -932,8 +1478,42 @@
         <f t="shared" si="1"/>
         <v>0.25080000000000002</v>
       </c>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M18" s="2">
+        <v>1.46E-2</v>
+      </c>
+      <c r="Q18" s="2">
+        <v>1.5599999999999999E-2</v>
+      </c>
+      <c r="R18" s="13">
+        <v>1.2800000000000001E-2</v>
+      </c>
+      <c r="S18">
+        <f t="shared" si="2"/>
+        <v>-6.8500000000000005E-2</v>
+      </c>
+      <c r="T18">
+        <f t="shared" si="3"/>
+        <v>0.12330000000000001</v>
+      </c>
+      <c r="W18" s="2">
+        <v>1.46E-2</v>
+      </c>
+      <c r="AA18" s="2">
+        <v>1.7500000000000002E-2</v>
+      </c>
+      <c r="AB18" s="2">
+        <v>1.43E-2</v>
+      </c>
+      <c r="AC18">
+        <f t="shared" si="4"/>
+        <v>-0.1986</v>
+      </c>
+      <c r="AD18">
+        <f t="shared" si="5"/>
+        <v>2.0500000000000001E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="3">
         <v>5.8100000000000003E-4</v>
       </c>
@@ -954,8 +1534,42 @@
         <f t="shared" si="1"/>
         <v>0.56110000000000004</v>
       </c>
-    </row>
-    <row r="20" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M19" s="4">
+        <v>7.3000000000000001E-3</v>
+      </c>
+      <c r="Q19" s="4">
+        <v>1.2500000000000001E-2</v>
+      </c>
+      <c r="R19" s="4">
+        <v>2.35E-2</v>
+      </c>
+      <c r="S19">
+        <f t="shared" si="2"/>
+        <v>-0.71230000000000004</v>
+      </c>
+      <c r="T19">
+        <f t="shared" si="3"/>
+        <v>-2.2191999999999998</v>
+      </c>
+      <c r="W19" s="4">
+        <v>7.3000000000000001E-3</v>
+      </c>
+      <c r="AA19" s="4">
+        <v>9.4999999999999998E-3</v>
+      </c>
+      <c r="AB19" s="11">
+        <v>6.4000000000000003E-3</v>
+      </c>
+      <c r="AC19">
+        <f t="shared" si="4"/>
+        <v>-0.3014</v>
+      </c>
+      <c r="AD19">
+        <f t="shared" si="5"/>
+        <v>0.12330000000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="4">
         <v>8.8999999999999995E-5</v>
       </c>
@@ -976,8 +1590,42 @@
         <f t="shared" si="1"/>
         <v>-1.9887999999999999</v>
       </c>
-    </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M20" s="5">
+        <v>7.6E-3</v>
+      </c>
+      <c r="Q20" s="5">
+        <v>1.0800000000000001E-2</v>
+      </c>
+      <c r="R20" s="5">
+        <v>1.29E-2</v>
+      </c>
+      <c r="S20">
+        <f t="shared" si="2"/>
+        <v>-0.42109999999999997</v>
+      </c>
+      <c r="T20">
+        <f t="shared" si="3"/>
+        <v>-0.69740000000000002</v>
+      </c>
+      <c r="W20" s="5">
+        <v>7.6E-3</v>
+      </c>
+      <c r="AA20" s="5">
+        <v>9.4000000000000004E-3</v>
+      </c>
+      <c r="AB20" s="14">
+        <v>6.4999999999999997E-3</v>
+      </c>
+      <c r="AC20">
+        <f t="shared" si="4"/>
+        <v>-0.23680000000000001</v>
+      </c>
+      <c r="AD20">
+        <f t="shared" si="5"/>
+        <v>0.1447</v>
+      </c>
+    </row>
+    <row r="21" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B21" s="1">
         <v>1.3899999999999999E-2</v>
       </c>
@@ -998,8 +1646,42 @@
         <f t="shared" si="1"/>
         <v>0.11509999999999999</v>
       </c>
-    </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M21" s="6">
+        <v>9.1999999999999998E-3</v>
+      </c>
+      <c r="Q21" s="6">
+        <v>1.0800000000000001E-2</v>
+      </c>
+      <c r="R21" s="15">
+        <v>8.3999999999999995E-3</v>
+      </c>
+      <c r="S21">
+        <f t="shared" si="2"/>
+        <v>-0.1739</v>
+      </c>
+      <c r="T21">
+        <f t="shared" si="3"/>
+        <v>8.6999999999999994E-2</v>
+      </c>
+      <c r="W21" s="6">
+        <v>9.1999999999999998E-3</v>
+      </c>
+      <c r="AA21" s="6">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="AB21" s="6">
+        <v>9.1000000000000004E-3</v>
+      </c>
+      <c r="AC21">
+        <f t="shared" si="4"/>
+        <v>-0.41299999999999998</v>
+      </c>
+      <c r="AD21">
+        <f t="shared" si="5"/>
+        <v>1.09E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="2">
         <v>1.4800000000000001E-2</v>
       </c>
@@ -1020,8 +1702,42 @@
         <f t="shared" si="1"/>
         <v>0.15540000000000001</v>
       </c>
-    </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M22" s="8">
+        <v>6.1999999999999998E-3</v>
+      </c>
+      <c r="Q22" s="8">
+        <v>1.03E-2</v>
+      </c>
+      <c r="R22" s="8">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="S22">
+        <f t="shared" si="2"/>
+        <v>-0.6613</v>
+      </c>
+      <c r="T22">
+        <f t="shared" si="3"/>
+        <v>-1.9032</v>
+      </c>
+      <c r="W22" s="8">
+        <v>6.1999999999999998E-3</v>
+      </c>
+      <c r="AA22" s="8">
+        <v>7.9000000000000008E-3</v>
+      </c>
+      <c r="AB22" s="12">
+        <v>4.4999999999999997E-3</v>
+      </c>
+      <c r="AC22">
+        <f t="shared" si="4"/>
+        <v>-0.2742</v>
+      </c>
+      <c r="AD22">
+        <f t="shared" si="5"/>
+        <v>0.2742</v>
+      </c>
+    </row>
+    <row r="23" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B23" s="3">
         <v>1.6400000000000001E-2</v>
       </c>
@@ -1043,7 +1759,7 @@
         <v>0.22559999999999999</v>
       </c>
     </row>
-    <row r="24" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="11">
         <v>7.6E-3</v>
       </c>
@@ -1064,8 +1780,20 @@
         <f t="shared" si="1"/>
         <v>-0.53949999999999998</v>
       </c>
-    </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M24" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>10</v>
+      </c>
+      <c r="R24" t="s">
+        <v>11</v>
+      </c>
+      <c r="W24" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B25" s="5">
         <v>0.01</v>
       </c>
@@ -1086,8 +1814,42 @@
         <f t="shared" si="1"/>
         <v>0.16</v>
       </c>
-    </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M25" s="1">
+        <v>3.5E-4</v>
+      </c>
+      <c r="Q25" s="1">
+        <v>2.5999999999999998E-4</v>
+      </c>
+      <c r="R25" s="1">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="S25">
+        <f t="shared" si="2"/>
+        <v>0.2571</v>
+      </c>
+      <c r="T25">
+        <f t="shared" si="3"/>
+        <v>-1.1429</v>
+      </c>
+      <c r="W25" s="1">
+        <v>3.5E-4</v>
+      </c>
+      <c r="AA25" s="1">
+        <v>2.3000000000000001E-4</v>
+      </c>
+      <c r="AB25" s="9">
+        <v>2.5000000000000001E-4</v>
+      </c>
+      <c r="AC25">
+        <f t="shared" si="4"/>
+        <v>0.34289999999999998</v>
+      </c>
+      <c r="AD25">
+        <f t="shared" si="5"/>
+        <v>0.28570000000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B26" s="6">
         <v>8.9999999999999993E-3</v>
       </c>
@@ -1108,8 +1870,42 @@
         <f t="shared" si="1"/>
         <v>0.18890000000000001</v>
       </c>
-    </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M26" s="13">
+        <v>3.4000000000000002E-4</v>
+      </c>
+      <c r="Q26" s="2">
+        <v>3.6000000000000002E-4</v>
+      </c>
+      <c r="R26" s="2">
+        <v>4.8999999999999998E-4</v>
+      </c>
+      <c r="S26">
+        <f t="shared" si="2"/>
+        <v>-5.8799999999999998E-2</v>
+      </c>
+      <c r="T26">
+        <f t="shared" si="3"/>
+        <v>-0.44119999999999998</v>
+      </c>
+      <c r="W26" s="13">
+        <v>3.4000000000000002E-4</v>
+      </c>
+      <c r="AA26" s="2">
+        <v>5.5000000000000003E-4</v>
+      </c>
+      <c r="AB26" s="2">
+        <v>3.6999999999999999E-4</v>
+      </c>
+      <c r="AC26">
+        <f t="shared" si="4"/>
+        <v>-0.61760000000000004</v>
+      </c>
+      <c r="AD26">
+        <f t="shared" si="5"/>
+        <v>-8.8200000000000001E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="7">
         <v>9.7999999999999997E-3</v>
       </c>
@@ -1130,8 +1926,42 @@
         <f t="shared" si="1"/>
         <v>0.1837</v>
       </c>
-    </row>
-    <row r="28" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M27" s="4">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="Q27" s="4">
+        <v>1.8000000000000001E-4</v>
+      </c>
+      <c r="R27" s="4">
+        <v>1.0200000000000001E-3</v>
+      </c>
+      <c r="S27">
+        <f t="shared" si="2"/>
+        <v>0.1</v>
+      </c>
+      <c r="T27">
+        <f t="shared" si="3"/>
+        <v>-4.0999999999999996</v>
+      </c>
+      <c r="W27" s="4">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="AA27" s="4">
+        <v>1E-4</v>
+      </c>
+      <c r="AB27" s="11">
+        <v>6.9999999999999994E-5</v>
+      </c>
+      <c r="AC27">
+        <f t="shared" si="4"/>
+        <v>0.5</v>
+      </c>
+      <c r="AD27">
+        <f t="shared" si="5"/>
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="28" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="12">
         <v>6.0000000000000001E-3</v>
       </c>
@@ -1152,8 +1982,78 @@
         <f t="shared" si="1"/>
         <v>-0.51670000000000005</v>
       </c>
-    </row>
-    <row r="30" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M28" s="1">
+        <v>1.49E-2</v>
+      </c>
+      <c r="Q28" s="1">
+        <v>1.4E-2</v>
+      </c>
+      <c r="R28" s="1">
+        <v>1.7299999999999999E-2</v>
+      </c>
+      <c r="S28">
+        <f t="shared" si="2"/>
+        <v>6.0400000000000002E-2</v>
+      </c>
+      <c r="T28">
+        <f t="shared" si="3"/>
+        <v>-0.16109999999999999</v>
+      </c>
+      <c r="W28" s="1">
+        <v>1.49E-2</v>
+      </c>
+      <c r="AA28" s="1">
+        <v>1.1900000000000001E-2</v>
+      </c>
+      <c r="AB28" s="1">
+        <v>9.9000000000000008E-3</v>
+      </c>
+      <c r="AC28">
+        <f t="shared" si="4"/>
+        <v>0.20130000000000001</v>
+      </c>
+      <c r="AD28">
+        <f t="shared" si="5"/>
+        <v>0.33560000000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="M29" s="2">
+        <v>1.5599999999999999E-2</v>
+      </c>
+      <c r="Q29" s="2">
+        <v>1.5599999999999999E-2</v>
+      </c>
+      <c r="R29" s="13">
+        <v>1.2800000000000001E-2</v>
+      </c>
+      <c r="S29">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T29">
+        <f t="shared" si="3"/>
+        <v>0.17949999999999999</v>
+      </c>
+      <c r="W29" s="2">
+        <v>1.5599999999999999E-2</v>
+      </c>
+      <c r="AA29" s="2">
+        <v>1.7500000000000002E-2</v>
+      </c>
+      <c r="AB29" s="2">
+        <v>1.43E-2</v>
+      </c>
+      <c r="AC29">
+        <f t="shared" si="4"/>
+        <v>-0.12180000000000001</v>
+      </c>
+      <c r="AD29">
+        <f t="shared" si="5"/>
+        <v>8.3299999999999999E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>4</v>
       </c>
@@ -1163,8 +2063,42 @@
       <c r="H30" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M30" s="4">
+        <v>1.3599999999999999E-2</v>
+      </c>
+      <c r="Q30" s="4">
+        <v>1.2500000000000001E-2</v>
+      </c>
+      <c r="R30" s="4">
+        <v>2.35E-2</v>
+      </c>
+      <c r="S30">
+        <f t="shared" si="2"/>
+        <v>8.09E-2</v>
+      </c>
+      <c r="T30">
+        <f t="shared" si="3"/>
+        <v>-0.72789999999999999</v>
+      </c>
+      <c r="W30" s="4">
+        <v>1.3599999999999999E-2</v>
+      </c>
+      <c r="AA30" s="4">
+        <v>9.4999999999999998E-3</v>
+      </c>
+      <c r="AB30" s="11">
+        <v>6.4000000000000003E-3</v>
+      </c>
+      <c r="AC30">
+        <f t="shared" si="4"/>
+        <v>0.30149999999999999</v>
+      </c>
+      <c r="AD30">
+        <f t="shared" si="5"/>
+        <v>0.52939999999999998</v>
+      </c>
+    </row>
+    <row r="31" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B31" s="1">
         <v>2.4399999999999999E-4</v>
       </c>
@@ -1185,8 +2119,42 @@
         <f t="shared" si="1"/>
         <v>-0.13519999999999999</v>
       </c>
-    </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M31" s="5">
+        <v>1.2200000000000001E-2</v>
+      </c>
+      <c r="Q31" s="5">
+        <v>1.0800000000000001E-2</v>
+      </c>
+      <c r="R31" s="5">
+        <v>1.29E-2</v>
+      </c>
+      <c r="S31">
+        <f t="shared" si="2"/>
+        <v>0.1148</v>
+      </c>
+      <c r="T31">
+        <f t="shared" si="3"/>
+        <v>-5.74E-2</v>
+      </c>
+      <c r="W31" s="5">
+        <v>1.2200000000000001E-2</v>
+      </c>
+      <c r="AA31" s="5">
+        <v>9.4000000000000004E-3</v>
+      </c>
+      <c r="AB31" s="14">
+        <v>6.4999999999999997E-3</v>
+      </c>
+      <c r="AC31">
+        <f t="shared" si="4"/>
+        <v>0.22950000000000001</v>
+      </c>
+      <c r="AD31">
+        <f t="shared" si="5"/>
+        <v>0.4672</v>
+      </c>
+    </row>
+    <row r="32" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B32" s="2">
         <v>2.7599999999999999E-4</v>
       </c>
@@ -1207,8 +2175,42 @@
         <f t="shared" si="1"/>
         <v>0.1123</v>
       </c>
-    </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M32" s="6">
+        <v>1.18E-2</v>
+      </c>
+      <c r="Q32" s="6">
+        <v>1.0800000000000001E-2</v>
+      </c>
+      <c r="R32" s="15">
+        <v>8.3999999999999995E-3</v>
+      </c>
+      <c r="S32">
+        <f t="shared" si="2"/>
+        <v>8.4699999999999998E-2</v>
+      </c>
+      <c r="T32">
+        <f t="shared" si="3"/>
+        <v>0.28810000000000002</v>
+      </c>
+      <c r="W32" s="6">
+        <v>1.18E-2</v>
+      </c>
+      <c r="AA32" s="6">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="AB32" s="6">
+        <v>9.1000000000000004E-3</v>
+      </c>
+      <c r="AC32">
+        <f t="shared" si="4"/>
+        <v>-0.1017</v>
+      </c>
+      <c r="AD32">
+        <f t="shared" si="5"/>
+        <v>0.2288</v>
+      </c>
+    </row>
+    <row r="33" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="3">
         <v>3.6099999999999999E-4</v>
       </c>
@@ -1229,8 +2231,42 @@
         <f t="shared" si="1"/>
         <v>0.29360000000000003</v>
       </c>
-    </row>
-    <row r="34" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M33" s="8">
+        <v>1.2200000000000001E-2</v>
+      </c>
+      <c r="Q33" s="8">
+        <v>1.03E-2</v>
+      </c>
+      <c r="R33" s="8">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="S33">
+        <f t="shared" si="2"/>
+        <v>0.15570000000000001</v>
+      </c>
+      <c r="T33">
+        <f t="shared" si="3"/>
+        <v>-0.47539999999999999</v>
+      </c>
+      <c r="W33" s="8">
+        <v>1.2200000000000001E-2</v>
+      </c>
+      <c r="AA33" s="8">
+        <v>7.9000000000000008E-3</v>
+      </c>
+      <c r="AB33" s="12">
+        <v>4.4999999999999997E-3</v>
+      </c>
+      <c r="AC33">
+        <f t="shared" si="4"/>
+        <v>0.35249999999999998</v>
+      </c>
+      <c r="AD33">
+        <f t="shared" si="5"/>
+        <v>0.63109999999999999</v>
+      </c>
+    </row>
+    <row r="34" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B34" s="4">
         <v>1.6699999999999999E-4</v>
       </c>
@@ -1252,7 +2288,7 @@
         <v>-0.59279999999999999</v>
       </c>
     </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B35" s="1">
         <v>1.47E-2</v>
       </c>
@@ -1274,7 +2310,7 @@
         <v>0.1633</v>
       </c>
     </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B36" s="2">
         <v>1.6E-2</v>
       </c>
@@ -1296,7 +2332,7 @@
         <v>0.21879999999999999</v>
       </c>
     </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B37" s="3">
         <v>1.7000000000000001E-2</v>
       </c>
@@ -1318,7 +2354,7 @@
         <v>0.25290000000000001</v>
       </c>
     </row>
-    <row r="38" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B38" s="4">
         <v>1.29E-2</v>
       </c>
@@ -1340,7 +2376,7 @@
         <v>9.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B39" s="5">
         <v>1.2500000000000001E-2</v>
       </c>
@@ -1362,7 +2398,7 @@
         <v>0.32800000000000001</v>
       </c>
     </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B40" s="6">
         <v>1.21E-2</v>
       </c>
@@ -1384,7 +2420,7 @@
         <v>0.3967</v>
       </c>
     </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B41" s="7">
         <v>1.24E-2</v>
       </c>
@@ -1406,7 +2442,7 @@
         <v>0.3548</v>
       </c>
     </row>
-    <row r="42" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B42" s="8">
         <v>1.23E-2</v>
       </c>
@@ -1430,18 +2466,26 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D3:D42">
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="6" priority="5" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J3:J42">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S3:T33 AC3:AD33">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>